<commit_message>
dew docs  and matlab experiments
</commit_message>
<xml_diff>
--- a/marketsai/experiments_log.xlsx
+++ b/marketsai/experiments_log.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matiascovarrubias/Documents/universidad/NYU/Research/Repositories/marketsAI/marketsai/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{971E0403-CD18-184C-B619-27947F63FFE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41DF3617-619F-F542-A79F-E842AC044E9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-51200" yWindow="-1040" windowWidth="51200" windowHeight="28340" activeTab="2" xr2:uid="{7A68A33C-84AE-7149-97C7-7F01ADCDFDEB}"/>
+    <workbookView xWindow="-51200" yWindow="-1040" windowWidth="51200" windowHeight="28340" xr2:uid="{7A68A33C-84AE-7149-97C7-7F01ADCDFDEB}"/>
   </bookViews>
   <sheets>
     <sheet name="expers_log" sheetId="6" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="80">
   <si>
     <t>Batch</t>
   </si>
@@ -259,6 +259,24 @@
   </si>
   <si>
     <t>Learned Policy</t>
+  </si>
+  <si>
+    <t>run 300 iteration of 5m batches on 1hh_planner_ma on server</t>
+  </si>
+  <si>
+    <t>/Users/matiascovarrubias/ray_results/native_1hh_capital_planner_ma_run_August16_PPO/PPO_capital_planner_ma_028d6_00000_0_2021-08-16_19-52-27/checkpoint_000300/checkpoint-300</t>
+  </si>
+  <si>
+    <t>run 300 iteration of 5m batches on 2hh_planner_ma on server</t>
+  </si>
+  <si>
+    <t>run 300 iteration of 5m batches on 3hh_planner_ma on server</t>
+  </si>
+  <si>
+    <t>run 300 iteration of 5m batches on 4hh_planner_ma on server</t>
+  </si>
+  <si>
+    <t>run 300 iteration of 5m batches on 5hh_planner_ma on server</t>
   </si>
 </sst>
 </file>
@@ -22007,15 +22025,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9AAE129-42DA-5B41-8861-66C3E3A905F9}">
-  <dimension ref="C4:F22"/>
+  <dimension ref="C4:F27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="3" max="3" width="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="63.5" style="6" customWidth="1"/>
     <col min="6" max="6" width="114" style="6" customWidth="1"/>
   </cols>
@@ -22245,6 +22263,61 @@
       </c>
       <c r="F22" s="7" t="s">
         <v>67</v>
+      </c>
+    </row>
+    <row r="23" spans="3:6" ht="34">
+      <c r="C23" s="4">
+        <v>44424</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="24" spans="3:6" ht="34">
+      <c r="C24" s="4">
+        <v>44424</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="25" spans="3:6" ht="34">
+      <c r="C25" s="4">
+        <v>44424</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="26" spans="3:6" ht="34">
+      <c r="C26" s="4">
+        <v>44424</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="F26" s="6" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="27" spans="3:6" ht="34">
+      <c r="C27" s="4">
+        <v>44424</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -22278,7 +22351,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE533DBA-7CCB-AA49-A9B0-5350D7585E08}">
   <dimension ref="A1:AQ304"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AE21" workbookViewId="0">
+    <sheetView topLeftCell="AE20" workbookViewId="0">
       <selection activeCell="AP3" sqref="AP3"/>
     </sheetView>
   </sheetViews>

</xml_diff>